<commit_message>
Input Error Fixing, STEP 5 Complete, Remove Feat
</commit_message>
<xml_diff>
--- a/Sources/test.xlsx
+++ b/Sources/test.xlsx
@@ -5,7 +5,7 @@
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPP2409-P\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
@@ -24,6 +24,12 @@
     <x:t>Shoulder</x:t>
   </x:si>
   <x:si>
+    <x:t>Leg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>week2</x:t>
+  </x:si>
+  <x:si>
     <x:t>week1</x:t>
   </x:si>
   <x:si>
@@ -37,12 +43,6 @@
   </x:si>
   <x:si>
     <x:t>week</x:t>
-  </x:si>
-  <x:si>
-    <x:t>week2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Leg</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -438,8 +438,8 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A1:E4"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <x:selection activeCell="F4" activeCellId="0" sqref="F4:F4"/>
+    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <x:selection activeCell="C6" activeCellId="0" sqref="C5:C6"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="16.39999999999999857891"/>
@@ -449,24 +449,24 @@
   <x:sheetData>
     <x:row r="1" spans="1:5">
       <x:c r="A1" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B1" t="s">
-        <x:v>7</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C1" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="D1" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="E1" t="s">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="A2" t="s">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2">
         <x:v>6200</x:v>
@@ -483,13 +483,10 @@
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="A3" t="s">
-        <x:v>6</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B3">
         <x:v>6540</x:v>
-      </x:c>
-      <x:c r="C3">
-        <x:v>3777</x:v>
       </x:c>
       <x:c r="D3">
         <x:v>5507</x:v>
@@ -500,7 +497,7 @@
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="A4" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="B4">
         <x:v>4360</x:v>
@@ -516,7 +513,7 @@
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:pageMargins left="0.74805557727813720703" right="0.74805557727813720703" top="0.98430556058883666992" bottom="0.98430556058883666992" header="0.51180553436279296875" footer="0.51180553436279296875"/>
+  <x:pageMargins left="0.74805557727813720703" right="0.74805557727813720703" top="0.98430556058883666992" bottom="0.98430556058883666992" header="0.51166665554046630859" footer="0.51166665554046630859"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
   <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="1"/>
 </x:worksheet>

</xml_diff>